<commit_message>
predator list with sizes
</commit_message>
<xml_diff>
--- a/data-raw/Table3.xlsx
+++ b/data-raw/Table3.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11012"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brian.smith\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sarah.gaichas/Documents/0_Data/benthosindex/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20FF3ADC-F2FE-E440-983C-1379BD88CB58}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11700"/>
+    <workbookView xWindow="31060" yWindow="-19240" windowWidth="17200" windowHeight="18920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SpTable" sheetId="1" r:id="rId1"/>
@@ -203,9 +204,6 @@
     <t>Melanogrammus aeglefinus</t>
   </si>
   <si>
-    <t>Polock</t>
-  </si>
-  <si>
     <t>Pollachius virens</t>
   </si>
   <si>
@@ -281,9 +279,6 @@
     <t>Glyptocephalus cynoglossus</t>
   </si>
   <si>
-    <t>Windowpane flounder</t>
-  </si>
-  <si>
     <t>Scophthalmus aquosus</t>
   </si>
   <si>
@@ -456,12 +451,18 @@
   </si>
   <si>
     <t>Loligo pealeii</t>
+  </si>
+  <si>
+    <t>Pollock</t>
+  </si>
+  <si>
+    <t>Windowpane</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -522,10 +523,6 @@
   </cellStyleXfs>
   <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -544,6 +541,10 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -823,1404 +824,1404 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:K55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.85546875" customWidth="1"/>
-    <col min="8" max="8" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.83203125" customWidth="1"/>
+    <col min="8" max="8" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="D2" s="1" t="s">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="D2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="B3" s="3" t="s">
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.15">
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="H3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="K3" s="5"/>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K3" s="3"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A4">
         <v>1</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="9" t="s">
+      <c r="D4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="9" t="s">
+      <c r="F4" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="G4" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H4" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A5">
         <v>2</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="9" t="s">
+      <c r="D5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="9" t="s">
+      <c r="F5" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="G5" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H5" s="7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A6">
         <v>3</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E6" s="9" t="s">
+      <c r="D6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="9" t="s">
+      <c r="F6" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="G6" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="9" t="s">
+      <c r="H6" s="7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A7">
         <v>4</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E7" s="9" t="s">
+      <c r="D7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="9" t="s">
+      <c r="F7" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="G7" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H7" s="9" t="s">
+      <c r="H7" s="7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A8">
         <v>5</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="9" t="s">
+      <c r="D8" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="9" t="s">
+      <c r="F8" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="G8" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H8" s="9" t="s">
+      <c r="H8" s="7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A9">
         <v>6</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D9" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="9" t="s">
+      <c r="D9" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E9" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="F9" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G9" s="9" t="s">
+      <c r="G9" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H9" s="9" t="s">
+      <c r="H9" s="7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A10">
         <v>7</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E10" s="9" t="s">
+      <c r="D10" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="F10" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G10" s="9" t="s">
+      <c r="G10" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H10" s="9" t="s">
+      <c r="H10" s="7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A11">
         <v>8</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E11" s="9" t="s">
+      <c r="D11" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E11" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="F11" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G11" s="9" t="s">
+      <c r="G11" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H11" s="9" t="s">
+      <c r="H11" s="7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A12">
         <v>9</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D12" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E12" s="9" t="s">
+      <c r="D12" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E12" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="F12" s="9" t="s">
+      <c r="F12" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G12" s="9" t="s">
+      <c r="G12" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H12" s="9" t="s">
+      <c r="H12" s="7" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A13">
         <v>10</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="E13" s="10" t="s">
+      <c r="E13" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="F13" s="10" t="s">
+      <c r="F13" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="G13" s="10" t="s">
+      <c r="G13" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="H13" s="10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H13" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A14">
         <v>11</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D14" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="E14" s="10" t="s">
+      <c r="E14" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="F14" s="10" t="s">
+      <c r="F14" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="G14" s="10" t="s">
+      <c r="G14" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="H14" s="10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H14" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A15">
         <v>12</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="D15" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="E15" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="F15" s="10" t="s">
+      <c r="F15" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="G15" s="10" t="s">
+      <c r="G15" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="H15" s="10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="H15" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.15">
       <c r="A16">
         <v>13</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D16" s="10" t="s">
+      <c r="D16" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="E16" s="10" t="s">
+      <c r="E16" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="F16" s="10" t="s">
+      <c r="F16" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="G16" s="10" t="s">
+      <c r="G16" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="H16" s="10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H16" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A17">
         <v>14</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D17" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E17" s="10" t="s">
+      <c r="D17" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="F17" s="10" t="s">
+      <c r="F17" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="G17" s="10" t="s">
+      <c r="G17" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="H17" s="10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H17" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A18">
         <v>15</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C18" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D18" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E18" s="10" t="s">
+      <c r="D18" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="F18" s="10" t="s">
+      <c r="F18" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="G18" s="10" t="s">
+      <c r="G18" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="H18" s="10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H18" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A19">
         <v>16</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="D19" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E19" s="10" t="s">
+      <c r="D19" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="F19" s="10" t="s">
+      <c r="F19" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="G19" s="10" t="s">
+      <c r="G19" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="H19" s="10" t="s">
+      <c r="H19" s="8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A20">
         <v>17</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="D20" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E20" s="10" t="s">
+      <c r="D20" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="F20" s="10" t="s">
+      <c r="F20" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="G20" s="10" t="s">
+      <c r="G20" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="H20" s="10" t="s">
+      <c r="H20" s="8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A21">
         <v>18</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C21" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E21" s="10" t="s">
+      <c r="D21" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="F21" s="10" t="s">
+      <c r="F21" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="G21" s="10" t="s">
+      <c r="G21" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="H21" s="10" t="s">
+      <c r="H21" s="8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A22">
         <v>19</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C22" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C22" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E22" s="10" t="s">
+      <c r="D22" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="F22" s="10" t="s">
+      <c r="F22" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="G22" s="10" t="s">
+      <c r="G22" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="H22" s="10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H22" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A23">
         <v>20</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C23" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C23" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E23" s="10" t="s">
+      <c r="D23" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="F23" s="10" t="s">
+      <c r="F23" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="G23" s="10" t="s">
+      <c r="G23" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="H23" s="10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H23" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A24">
         <v>21</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C24" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C24" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E24" s="10" t="s">
+      <c r="D24" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="F24" s="10" t="s">
+      <c r="F24" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="G24" s="10" t="s">
+      <c r="G24" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="H24" s="10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H24" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A25">
         <v>22</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C25" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="D25" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F25" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G25" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="D25" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E25" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="F25" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="G25" s="10" t="s">
+      <c r="H25" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="H25" s="10" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A26">
         <v>23</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B26" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="C26" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="C26" s="7" t="s">
+      <c r="D26" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="G26" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="D26" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E26" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="F26" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="G26" s="10" t="s">
+      <c r="H26" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="H26" s="10" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A27">
         <v>24</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C27" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="C27" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="D27" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E27" s="10" t="s">
+      <c r="D27" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="F27" s="10" t="s">
+      <c r="F27" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="G27" s="10" t="s">
+      <c r="G27" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="H27" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="H27" s="10" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A28">
         <v>25</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C28" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="C28" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="D28" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E28" s="10" t="s">
+      <c r="D28" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E28" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="F28" s="10" t="s">
+      <c r="F28" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="G28" s="10" t="s">
+      <c r="G28" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="H28" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="H28" s="10" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A29">
         <v>26</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B29" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C29" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="C29" s="7" t="s">
-        <v>80</v>
-      </c>
-      <c r="D29" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E29" s="10" t="s">
+      <c r="D29" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="F29" s="10" t="s">
+      <c r="F29" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="G29" s="10" t="s">
+      <c r="G29" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="H29" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="H29" s="10" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A30">
         <v>27</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B30" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C30" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="C30" s="7" t="s">
-        <v>82</v>
-      </c>
-      <c r="D30" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E30" s="10" t="s">
+      <c r="D30" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E30" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="F30" s="10" t="s">
+      <c r="F30" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="G30" s="10" t="s">
+      <c r="G30" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="H30" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="H30" s="10" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A31">
         <v>28</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="B31" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C31" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C31" s="7" t="s">
-        <v>84</v>
-      </c>
-      <c r="D31" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E31" s="10" t="s">
+      <c r="D31" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E31" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="F31" s="10" t="s">
+      <c r="F31" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="G31" s="10" t="s">
+      <c r="G31" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="H31" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="H31" s="10" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A32">
         <v>29</v>
       </c>
-      <c r="B32" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="C32" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="D32" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E32" s="10" t="s">
+      <c r="B32" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E32" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="F32" s="10" t="s">
+      <c r="F32" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="G32" s="10" t="s">
+      <c r="G32" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="H32" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="H32" s="10" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A33">
         <v>30</v>
       </c>
-      <c r="B33" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="C33" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="D33" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E33" s="10" t="s">
+      <c r="B33" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E33" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="F33" s="10" t="s">
+      <c r="F33" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="G33" s="10" t="s">
+      <c r="G33" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="H33" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="H33" s="10" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A34">
         <v>31</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B34" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="F34" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="C34" s="7" t="s">
+      <c r="G34" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="D34" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="E34" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="F34" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="G34" s="10" t="s">
-        <v>92</v>
-      </c>
-      <c r="H34" s="10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H34" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A35">
         <v>32</v>
       </c>
-      <c r="B35" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="C35" s="7" t="s">
-        <v>94</v>
-      </c>
-      <c r="D35" s="10" t="s">
+      <c r="B35" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D35" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="E35" s="10" t="s">
+      <c r="E35" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="F35" s="10" t="s">
+      <c r="F35" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="G35" s="10" t="s">
+      <c r="G35" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="H35" s="10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H35" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A36">
         <v>33</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="B36" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F36" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="C36" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="D36" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E36" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="F36" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="G36" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="H36" s="10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G36" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="H36" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A37">
         <v>34</v>
       </c>
-      <c r="B37" s="6" t="s">
+      <c r="B37" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E37" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="C37" s="7" t="s">
+      <c r="F37" s="8" t="s">
         <v>99</v>
       </c>
-      <c r="D37" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E37" s="10" t="s">
+      <c r="G37" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="F37" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="G37" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="H37" s="10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H37" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A38">
         <v>35</v>
       </c>
-      <c r="B38" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="C38" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="D38" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E38" s="10" t="s">
+      <c r="B38" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E38" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F38" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="G38" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="H38" s="10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="F38" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="G38" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="H38" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A39">
         <v>36</v>
       </c>
-      <c r="B39" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="C39" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="D39" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E39" s="10" t="s">
+      <c r="B39" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="F39" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="G39" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="F39" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="G39" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="H39" s="10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H39" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A40">
         <v>37</v>
       </c>
-      <c r="B40" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="C40" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="D40" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E40" s="10" t="s">
+      <c r="B40" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E40" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="F40" s="10" t="s">
+      <c r="F40" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="G40" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="H40" s="10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G40" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="H40" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A41">
         <v>38</v>
       </c>
-      <c r="B41" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="C41" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="D41" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E41" s="10" t="s">
+      <c r="B41" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E41" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="F41" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="G41" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="F41" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="G41" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="H41" s="10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H41" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A42">
         <v>39</v>
       </c>
-      <c r="B42" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="C42" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="D42" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E42" s="10" t="s">
+      <c r="B42" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E42" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="F42" s="10" t="s">
+      <c r="F42" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="G42" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="H42" s="10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G42" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="H42" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A43">
         <v>40</v>
       </c>
-      <c r="B43" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="C43" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="D43" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E43" s="10" t="s">
+      <c r="B43" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E43" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="F43" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="G43" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="F43" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="G43" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="H43" s="10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H43" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A44">
         <v>41</v>
       </c>
-      <c r="B44" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="C44" s="7" t="s">
-        <v>116</v>
-      </c>
-      <c r="D44" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E44" s="10" t="s">
+      <c r="B44" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E44" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="F44" s="10" t="s">
+      <c r="F44" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="G44" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="H44" s="10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G44" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="H44" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A45">
         <v>42</v>
       </c>
-      <c r="B45" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="C45" s="7" t="s">
-        <v>118</v>
-      </c>
-      <c r="D45" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E45" s="10" t="s">
+      <c r="B45" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E45" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="F45" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="G45" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="F45" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="G45" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="H45" s="10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H45" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A46">
         <v>43</v>
       </c>
-      <c r="B46" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="C46" s="7" t="s">
-        <v>120</v>
-      </c>
-      <c r="D46" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E46" s="10" t="s">
+      <c r="B46" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E46" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="F46" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="G46" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="F46" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="G46" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="H46" s="10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H46" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A47">
         <v>44</v>
       </c>
-      <c r="B47" s="6" t="s">
-        <v>121</v>
-      </c>
-      <c r="C47" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="D47" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E47" s="10" t="s">
+      <c r="B47" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E47" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="F47" s="10" t="s">
+      <c r="F47" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="G47" s="10" t="s">
+      <c r="G47" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="H47" s="10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H47" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A48">
         <v>45</v>
       </c>
-      <c r="B48" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="C48" s="7" t="s">
-        <v>124</v>
-      </c>
-      <c r="D48" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E48" s="10" t="s">
+      <c r="B48" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E48" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="F48" s="10" t="s">
+      <c r="F48" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="G48" s="10" t="s">
+      <c r="G48" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="H48" s="10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H48" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A49">
         <v>46</v>
       </c>
-      <c r="B49" s="6" t="s">
+      <c r="B49" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E49" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="F49" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="C49" s="7" t="s">
+      <c r="G49" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="D49" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E49" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="F49" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="G49" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="H49" s="10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H49" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A50">
         <v>47</v>
       </c>
-      <c r="B50" s="6" t="s">
+      <c r="B50" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E50" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F50" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="G50" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="C50" s="7" t="s">
-        <v>130</v>
-      </c>
-      <c r="D50" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E50" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="F50" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="G50" s="10" t="s">
-        <v>131</v>
-      </c>
-      <c r="H50" s="10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H50" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A51">
         <v>48</v>
       </c>
-      <c r="B51" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="C51" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="D51" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E51" s="10" t="s">
+      <c r="B51" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E51" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="F51" s="10" t="s">
+      <c r="F51" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="G51" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="H51" s="10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G51" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="H51" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A52">
         <v>49</v>
       </c>
-      <c r="B52" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="C52" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="D52" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E52" s="10" t="s">
+      <c r="B52" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="D52" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E52" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F52" s="10" t="s">
+      <c r="F52" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="G52" s="10" t="s">
+      <c r="G52" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="H52" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="H52" s="10" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A53">
         <v>50</v>
       </c>
-      <c r="B53" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="C53" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="D53" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E53" s="10" t="s">
+      <c r="B53" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E53" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="F53" s="10" t="s">
+      <c r="F53" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="G53" s="10" t="s">
-        <v>102</v>
-      </c>
-      <c r="H53" s="10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="G53" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="H53" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A54">
         <v>51</v>
       </c>
-      <c r="B54" s="6" t="s">
+      <c r="B54" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E54" s="8" t="s">
         <v>138</v>
       </c>
-      <c r="C54" s="7" t="s">
+      <c r="F54" s="8" t="s">
         <v>139</v>
       </c>
-      <c r="D54" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E54" s="10" t="s">
-        <v>140</v>
-      </c>
-      <c r="F54" s="10" t="s">
-        <v>141</v>
-      </c>
-      <c r="G54" s="10" t="s">
+      <c r="G54" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="H54" s="10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H54" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A55">
         <v>52</v>
       </c>
-      <c r="B55" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="C55" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="D55" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="E55" s="10" t="s">
+      <c r="B55" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="F55" s="10" t="s">
+      <c r="C55" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="G55" s="10" t="s">
+      <c r="D55" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E55" s="8" t="s">
+        <v>138</v>
+      </c>
+      <c r="F55" s="8" t="s">
+        <v>139</v>
+      </c>
+      <c r="G55" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="H55" s="10" t="s">
+      <c r="H55" s="8" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>